<commit_message>
Excel Doc Complete (100%)
Change upon request on header content.
</commit_message>
<xml_diff>
--- a/excel/excelOrder97.xlsx
+++ b/excel/excelOrder97.xlsx
@@ -21,64 +21,52 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>[Sample:] James Johson</t>
+    <t>DK NY</t>
   </si>
   <si>
     <t>Data of Estimate:</t>
   </si>
   <si>
-    <t>[Sample:] 12.08.2014</t>
-  </si>
-  <si>
     <t>Sales Rep:</t>
   </si>
   <si>
-    <t>[Sample:] Company Repersentative</t>
-  </si>
-  <si>
     <t>Firm:</t>
   </si>
   <si>
-    <t>[Sample:] FIRM NAME INC</t>
-  </si>
-  <si>
     <t>Project Number:</t>
   </si>
   <si>
-    <t>[Sample:] P-0065</t>
-  </si>
-  <si>
     <t>Region:</t>
   </si>
   <si>
-    <t>[Sample:] EAST COAST</t>
-  </si>
-  <si>
     <t>Address:</t>
   </si>
   <si>
-    <t xml:space="preserve">[Sample:] 12345 N 100 Avenue </t>
+    <t>test@test.com</t>
   </si>
   <si>
     <t>Project Name:</t>
   </si>
   <si>
-    <t>[Sample:] TBD</t>
+    <t>Email</t>
   </si>
   <si>
     <t>Project Address:</t>
   </si>
   <si>
+    <t>affas</t>
+  </si>
+  <si>
     <t>Lead Time:</t>
   </si>
   <si>
-    <t>[Sample:] 8-10 WEEKS UPON ORDER APPROVAL AND RECEIPT OF DEPOSIT</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>[Sample:] 123-456-7890</t>
+    <t>8-10 WEEKS UPON ORDER APPROVAL AND RECEIPT OF DEPOSIT</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>afsfas</t>
   </si>
   <si>
     <t>ROOM</t>
@@ -154,6 +142,18 @@
   </si>
   <si>
     <t xml:space="preserve">1 BP </t>
+  </si>
+  <si>
+    <t>Kitchen</t>
+  </si>
+  <si>
+    <t>FE3008B-A1100010FF</t>
+  </si>
+  <si>
+    <t>Canon de Fusil Anthracite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 VV </t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="O8" sqref="O8"/>
@@ -522,554 +522,770 @@
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2"/>
+      <c r="L2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" t="s">
-        <v>5</v>
-      </c>
+      <c r="M2"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3"/>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3"/>
+      <c r="L3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" t="s">
-        <v>11</v>
-      </c>
+      <c r="M3"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="L5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="M5" t="s">
         <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B6"/>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9"/>
       <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
         <v>36</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" t="s">
-        <v>40</v>
-      </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J9">
         <v>3</v>
       </c>
       <c r="K9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10"/>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G10"/>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J10">
         <v>3</v>
       </c>
       <c r="K10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11"/>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G11"/>
       <c r="H11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J11">
         <v>3</v>
       </c>
       <c r="K11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12"/>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G12"/>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J12">
         <v>3</v>
       </c>
       <c r="K12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13"/>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G13"/>
       <c r="H13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J13">
         <v>3</v>
       </c>
       <c r="K13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J14">
         <v>7</v>
       </c>
       <c r="K14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15"/>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G15"/>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J15">
         <v>7</v>
       </c>
       <c r="K15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16"/>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J16">
         <v>7</v>
       </c>
       <c r="K16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17"/>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J17">
         <v>7</v>
       </c>
       <c r="K17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18"/>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J18">
         <v>7</v>
       </c>
       <c r="K18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" t="s">
         <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19">
+        <v>6</v>
+      </c>
+      <c r="K19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20">
+        <v>6</v>
+      </c>
+      <c r="K20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N20" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21"/>
+      <c r="H21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21">
+        <v>6</v>
+      </c>
+      <c r="K21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" t="s">
+        <v>35</v>
+      </c>
+      <c r="M21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22">
+        <v>6</v>
+      </c>
+      <c r="K22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" t="s">
+        <v>35</v>
+      </c>
+      <c r="M22" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23"/>
+      <c r="H23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23">
+        <v>6</v>
+      </c>
+      <c r="K23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" t="s">
+        <v>35</v>
+      </c>
+      <c r="M23" t="s">
+        <v>35</v>
+      </c>
+      <c r="N23" t="s">
+        <v>35</v>
+      </c>
+      <c r="O23" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>